<commit_message>
Modified and enhanced loaders.
</commit_message>
<xml_diff>
--- a/src/main/resources/Life management.xlsx
+++ b/src/main/resources/Life management.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="274">
   <si>
     <t>id</t>
   </si>
@@ -42,69 +42,69 @@
     <t>finish date</t>
   </si>
   <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>EPOCH1</t>
+  </si>
+  <si>
     <t>threads</t>
   </si>
   <si>
+    <t>Messinaissance</t>
+  </si>
+  <si>
+    <t>weave</t>
+  </si>
+  <si>
+    <t>EPOCH2</t>
+  </si>
+  <si>
+    <t>laser donuts</t>
+  </si>
+  <si>
+    <t>Sangenie</t>
+  </si>
+  <si>
+    <t>WEEK1</t>
+  </si>
+  <si>
+    <t>EPOCH3</t>
+  </si>
+  <si>
+    <t>Wakanda</t>
+  </si>
+  <si>
     <t>2016</t>
   </si>
   <si>
-    <t>EPOCH1</t>
+    <t>EPOCH4</t>
+  </si>
+  <si>
+    <t>Abyssinian Solar Empire</t>
+  </si>
+  <si>
+    <t>THREAD6</t>
   </si>
   <si>
     <t>THREAD1, THREAD2, THREAD3</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>Messinaissance</t>
-  </si>
-  <si>
-    <t>EPOCH2</t>
-  </si>
-  <si>
-    <t>Sangenie</t>
-  </si>
-  <si>
-    <t>EPOCH3</t>
-  </si>
-  <si>
-    <t>Wakanda</t>
-  </si>
-  <si>
-    <t>EPOCH4</t>
-  </si>
-  <si>
-    <t>Abyssinian Solar Empire</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>weave</t>
-  </si>
-  <si>
-    <t>laser donuts</t>
-  </si>
-  <si>
-    <t>WEEK1</t>
-  </si>
-  <si>
-    <t>THREAD6</t>
+    <t>WEAVE1</t>
+  </si>
+  <si>
+    <t>LD3</t>
   </si>
   <si>
     <t>week</t>
   </si>
   <si>
-    <t>WEAVE1</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
-    <t>LD3</t>
-  </si>
-  <si>
     <t>portion</t>
   </si>
   <si>
@@ -129,12 +129,12 @@
     <t>PORTION4</t>
   </si>
   <si>
+    <t>active hobby</t>
+  </si>
+  <si>
     <t>HOBBY3</t>
   </si>
   <si>
-    <t>active hobby</t>
-  </si>
-  <si>
     <t>SUNDAY1</t>
   </si>
   <si>
@@ -150,90 +150,90 @@
     <t>type</t>
   </si>
   <si>
+    <t>THEME1</t>
+  </si>
+  <si>
     <t>BL1</t>
   </si>
   <si>
+    <t>Adulthood</t>
+  </si>
+  <si>
+    <t>THEME2</t>
+  </si>
+  <si>
     <t>I don't know enough about Linux</t>
   </si>
   <si>
+    <t>Health</t>
+  </si>
+  <si>
     <t>Issue</t>
   </si>
   <si>
+    <t>THEME3</t>
+  </si>
+  <si>
     <t>BL2</t>
   </si>
   <si>
+    <t>Career Capital</t>
+  </si>
+  <si>
     <t>I want to be the best of the best at programming</t>
   </si>
   <si>
+    <t>THEME4</t>
+  </si>
+  <si>
+    <t>Mission</t>
+  </si>
+  <si>
     <t>BL3</t>
   </si>
   <si>
-    <t>THEME1</t>
+    <t>THEME5</t>
   </si>
   <si>
     <t>I want to lose fat</t>
   </si>
   <si>
-    <t>Adulthood</t>
+    <t>Passions</t>
   </si>
   <si>
     <t>BL4</t>
   </si>
   <si>
-    <t>THEME2</t>
-  </si>
-  <si>
     <t>I want to birth the 3rd iteration of television</t>
   </si>
   <si>
-    <t>Health</t>
-  </si>
-  <si>
     <t>Idea</t>
   </si>
   <si>
-    <t>THEME3</t>
+    <t>THEME6</t>
   </si>
   <si>
     <t>BL5</t>
   </si>
   <si>
-    <t>Career Capital</t>
-  </si>
-  <si>
-    <t>THEME4</t>
+    <t>Meta</t>
   </si>
   <si>
     <t>I need to get my shit together</t>
   </si>
   <si>
-    <t>Mission</t>
-  </si>
-  <si>
-    <t>THEME5</t>
-  </si>
-  <si>
     <t>BL6</t>
   </si>
   <si>
-    <t>Passions</t>
-  </si>
-  <si>
     <t>I need to become independent and self-reliant</t>
   </si>
   <si>
-    <t>THEME6</t>
-  </si>
-  <si>
     <t>BL7</t>
   </si>
   <si>
     <t>I am embarrased about not knowing how to cook</t>
   </si>
   <si>
-    <t>Meta</t>
-  </si>
-  <si>
     <t>BL8</t>
   </si>
   <si>
@@ -258,175 +258,343 @@
     <t>graduation</t>
   </si>
   <si>
+    <t>GOAL1</t>
+  </si>
+  <si>
+    <t>Buy a house</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>NotAchieved</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>GOAL2</t>
+  </si>
+  <si>
+    <t>BL6, BL7</t>
+  </si>
+  <si>
+    <t>Only eat food that you have cooked</t>
+  </si>
+  <si>
+    <t>Thread</t>
+  </si>
+  <si>
+    <t>GOAL3</t>
+  </si>
+  <si>
+    <t>BL6, BL8</t>
+  </si>
+  <si>
+    <t>Get a driving license</t>
+  </si>
+  <si>
+    <t>Goal</t>
+  </si>
+  <si>
+    <t>GOAL4</t>
+  </si>
+  <si>
+    <t>Learn DIY and repair</t>
+  </si>
+  <si>
+    <t>Hobby</t>
+  </si>
+  <si>
+    <t>GOAL5</t>
+  </si>
+  <si>
+    <t>Learn self-defence</t>
+  </si>
+  <si>
+    <t>GOAL6</t>
+  </si>
+  <si>
+    <t>Travel</t>
+  </si>
+  <si>
+    <t>GOAL7</t>
+  </si>
+  <si>
+    <t>Exercise your body</t>
+  </si>
+  <si>
+    <t>Employed</t>
+  </si>
+  <si>
+    <t>GOAL8</t>
+  </si>
+  <si>
+    <t>Exercise your mind</t>
+  </si>
+  <si>
+    <t>GOAL9</t>
+  </si>
+  <si>
+    <t>Eat well</t>
+  </si>
+  <si>
+    <t>GOAL10</t>
+  </si>
+  <si>
+    <t>Maintain hygiene</t>
+  </si>
+  <si>
+    <t>GOAL11</t>
+  </si>
+  <si>
+    <t>Sleep well</t>
+  </si>
+  <si>
+    <t>GOAL12</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>Weave</t>
+  </si>
+  <si>
     <t>goal</t>
   </si>
   <si>
-    <t>GOAL1</t>
-  </si>
-  <si>
-    <t>Buy a house</t>
+    <t>GOAL13</t>
+  </si>
+  <si>
+    <t>DevOps</t>
   </si>
   <si>
     <t>THREAD1</t>
   </si>
   <si>
-    <t>GOAL11</t>
+    <t>GOAL14</t>
+  </si>
+  <si>
+    <t>Configure build server</t>
   </si>
   <si>
     <t>Wake up</t>
   </si>
   <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Mobile Development</t>
+  </si>
+  <si>
+    <t>NotComplete</t>
+  </si>
+  <si>
     <t>NotStarted</t>
   </si>
   <si>
+    <t>WEAVE2</t>
+  </si>
+  <si>
     <t>THREAD2</t>
   </si>
   <si>
-    <t>GOAL7</t>
+    <t>GOAL25</t>
+  </si>
+  <si>
+    <t>Fix Martindale bug</t>
   </si>
   <si>
     <t>Go for a run</t>
   </si>
   <si>
+    <t>BAU</t>
+  </si>
+  <si>
+    <t>GOAL15</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
     <t>THREAD3</t>
   </si>
   <si>
-    <t>GOAL10</t>
+    <t>Software Architecture</t>
+  </si>
+  <si>
+    <t>GOAL28</t>
+  </si>
+  <si>
+    <t>Organise an Akka dojo</t>
   </si>
   <si>
     <t>Take a shower</t>
   </si>
   <si>
+    <t>PDR</t>
+  </si>
+  <si>
     <t>THREAD4</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>Sleep</t>
   </si>
   <si>
-    <t>NotComplete</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>GOAL2</t>
+    <t>GOAL16</t>
   </si>
   <si>
     <t>Clean your room</t>
   </si>
   <si>
-    <t>BL6, BL7</t>
+    <t>Cybersecurity</t>
   </si>
   <si>
     <t>Make your bed</t>
   </si>
   <si>
-    <t>Only eat food that you have cooked</t>
-  </si>
-  <si>
-    <t>GOAL13</t>
-  </si>
-  <si>
-    <t>Configure build server</t>
-  </si>
-  <si>
-    <t>Priority</t>
-  </si>
-  <si>
-    <t>WEAVE2</t>
-  </si>
-  <si>
-    <t>GOAL25</t>
-  </si>
-  <si>
-    <t>Fix Martindale bug</t>
-  </si>
-  <si>
-    <t>BAU</t>
-  </si>
-  <si>
-    <t>Complete</t>
-  </si>
-  <si>
-    <t>GOAL28</t>
-  </si>
-  <si>
-    <t>Organise an Akka dojo</t>
-  </si>
-  <si>
-    <t>PDR</t>
-  </si>
-  <si>
-    <t>Thread</t>
-  </si>
-  <si>
-    <t>GOAL3</t>
-  </si>
-  <si>
-    <t>BL6, BL8</t>
-  </si>
-  <si>
-    <t>Get a driving license</t>
-  </si>
-  <si>
-    <t>Goal</t>
-  </si>
-  <si>
-    <t>GOAL4</t>
-  </si>
-  <si>
-    <t>Learn DIY and repair</t>
-  </si>
-  <si>
-    <t>Hobby</t>
-  </si>
-  <si>
-    <t>GOAL5</t>
-  </si>
-  <si>
-    <t>Learn self-defence</t>
-  </si>
-  <si>
-    <t>GOAL6</t>
-  </si>
-  <si>
-    <t>Travel</t>
-  </si>
-  <si>
-    <t>Exercise your body</t>
-  </si>
-  <si>
-    <t>Employed</t>
-  </si>
-  <si>
-    <t>GOAL8</t>
-  </si>
-  <si>
-    <t>Exercise your mind</t>
-  </si>
-  <si>
-    <t>GOAL9</t>
-  </si>
-  <si>
-    <t>Eat well</t>
-  </si>
-  <si>
-    <t>Maintain hygiene</t>
+    <t>GOAL17</t>
+  </si>
+  <si>
+    <t>Big Data</t>
+  </si>
+  <si>
+    <t>GOAL18</t>
+  </si>
+  <si>
+    <t>UX Design</t>
+  </si>
+  <si>
+    <t>GOAL19</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>GOAL20</t>
+  </si>
+  <si>
+    <t>Database Technologies</t>
+  </si>
+  <si>
+    <t>GOAL21</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>GOAL22</t>
+  </si>
+  <si>
+    <t>Logical Reasoning</t>
+  </si>
+  <si>
+    <t>GOAL23</t>
+  </si>
+  <si>
+    <t>Maths</t>
+  </si>
+  <si>
+    <t>GOAL24</t>
+  </si>
+  <si>
+    <t>Algorithms &amp; Data-structures</t>
+  </si>
+  <si>
+    <t>Operating Systems</t>
+  </si>
+  <si>
+    <t>GOAL26</t>
+  </si>
+  <si>
+    <t>Building Compilers</t>
+  </si>
+  <si>
+    <t>GOAL27</t>
+  </si>
+  <si>
+    <t>Cryptography</t>
+  </si>
+  <si>
+    <t>Parallel Programming</t>
+  </si>
+  <si>
+    <t>GOAL29</t>
+  </si>
+  <si>
+    <t>Agile Methodology</t>
+  </si>
+  <si>
+    <t>GOAL30</t>
+  </si>
+  <si>
+    <t>Technical Writing</t>
+  </si>
+  <si>
+    <t>GOAL31</t>
+  </si>
+  <si>
+    <t>FinTech</t>
+  </si>
+  <si>
+    <t>GOAL32</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>GOAL33</t>
+  </si>
+  <si>
+    <t>The Sangenie</t>
+  </si>
+  <si>
+    <t>GOAL34</t>
+  </si>
+  <si>
+    <t>Master at least one foreign language</t>
+  </si>
+  <si>
+    <t>GOAL35</t>
+  </si>
+  <si>
+    <t>Master at least one sport</t>
+  </si>
+  <si>
+    <t>GOAL36</t>
+  </si>
+  <si>
+    <t>laser donut</t>
+  </si>
+  <si>
+    <t>Rekindle your artistic passion</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>PORTION1</t>
+  </si>
+  <si>
+    <t>LD2</t>
   </si>
   <si>
     <t>milestone</t>
   </si>
   <si>
-    <t>order</t>
+    <t>GOAL37</t>
+  </si>
+  <si>
+    <t>Create case classes</t>
+  </si>
+  <si>
+    <t>Learn to play an instrument</t>
   </si>
   <si>
     <t>LD1</t>
   </si>
   <si>
-    <t>Sleep well</t>
+    <t>PORTION2</t>
   </si>
   <si>
     <t>Search for a place to buy</t>
@@ -435,7 +603,10 @@
     <t>Search houses and flats in commuter towns</t>
   </si>
   <si>
-    <t>GOAL12</t>
+    <t>Represent basic functionalities for every type of item using case matching on SpokeType</t>
+  </si>
+  <si>
+    <t>GOAL38</t>
   </si>
   <si>
     <t>Make an offer</t>
@@ -444,13 +615,10 @@
     <t>ProjectBased</t>
   </si>
   <si>
-    <t>Coding</t>
-  </si>
-  <si>
-    <t>Weave</t>
-  </si>
-  <si>
-    <t>LD2</t>
+    <t>Read all of the books in your library, and blog about them</t>
+  </si>
+  <si>
+    <t>Create spreadsheets using the Abstract and the Career Capital list as references</t>
   </si>
   <si>
     <t>GOAL39</t>
@@ -459,19 +627,16 @@
     <t>Create a web-service</t>
   </si>
   <si>
-    <t>DevOps</t>
-  </si>
-  <si>
     <t>This should communicate with Neo4j and expose the data on an API</t>
   </si>
   <si>
     <t>A working pipeline</t>
   </si>
   <si>
-    <t>GOAL14</t>
-  </si>
-  <si>
-    <t>Mobile Development</t>
+    <t>Create a batch Scala project, that takes in an excel spreadsheet, communicates with LifeManager</t>
+  </si>
+  <si>
+    <t>Meditate</t>
   </si>
   <si>
     <t>Replicate the Conceptual Map</t>
@@ -480,204 +645,96 @@
     <t>Replicate the Conceptual Map inside the Ferris Wheel</t>
   </si>
   <si>
+    <t>GOAL40</t>
+  </si>
+  <si>
     <t>All data is on Neo4j</t>
   </si>
   <si>
-    <t>GOAL15</t>
-  </si>
-  <si>
-    <t>Software Architecture</t>
-  </si>
-  <si>
-    <t>GOAL16</t>
-  </si>
-  <si>
-    <t>Cybersecurity</t>
-  </si>
-  <si>
-    <t>GOAL17</t>
-  </si>
-  <si>
-    <t>Big Data</t>
-  </si>
-  <si>
-    <t>GOAL18</t>
-  </si>
-  <si>
-    <t>UX Design</t>
-  </si>
-  <si>
-    <t>GOAL19</t>
-  </si>
-  <si>
-    <t>Artificial Intelligence</t>
-  </si>
-  <si>
-    <t>GOAL20</t>
-  </si>
-  <si>
-    <t>Database Technologies</t>
-  </si>
-  <si>
-    <t>GOAL21</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>GOAL22</t>
-  </si>
-  <si>
-    <t>Logical Reasoning</t>
-  </si>
-  <si>
-    <t>GOAL23</t>
-  </si>
-  <si>
-    <t>Maths</t>
-  </si>
-  <si>
-    <t>laser donut</t>
-  </si>
-  <si>
-    <t>GOAL24</t>
-  </si>
-  <si>
-    <t>Algorithms &amp; Data-structures</t>
-  </si>
-  <si>
-    <t>PORTION1</t>
-  </si>
-  <si>
-    <t>Create case classes</t>
-  </si>
-  <si>
-    <t>Operating Systems</t>
-  </si>
-  <si>
-    <t>PORTION2</t>
-  </si>
-  <si>
-    <t>GOAL26</t>
-  </si>
-  <si>
-    <t>Represent basic functionalities for every type of item using case matching on SpokeType</t>
-  </si>
-  <si>
-    <t>Building Compilers</t>
-  </si>
-  <si>
-    <t>Create spreadsheets using the Abstract and the Career Capital list as references</t>
-  </si>
-  <si>
-    <t>GOAL27</t>
-  </si>
-  <si>
-    <t>Cryptography</t>
-  </si>
-  <si>
-    <t>Parallel Programming</t>
-  </si>
-  <si>
-    <t>Create a batch Scala project, that takes in an excel spreadsheet, communicates with LifeManager</t>
-  </si>
-  <si>
-    <t>GOAL29</t>
-  </si>
-  <si>
-    <t>Agile Methodology</t>
-  </si>
-  <si>
-    <t>GOAL30</t>
-  </si>
-  <si>
-    <t>Technical Writing</t>
-  </si>
-  <si>
-    <t>GOAL31</t>
-  </si>
-  <si>
-    <t>FinTech</t>
-  </si>
-  <si>
-    <t>GOAL32</t>
-  </si>
-  <si>
-    <t>Hardware</t>
-  </si>
-  <si>
     <t>TODO1</t>
   </si>
   <si>
-    <t>GOAL33</t>
+    <t>frequency</t>
   </si>
   <si>
     <t>Create a spreadsheet for Year</t>
   </si>
   <si>
+    <t>HOBBY1</t>
+  </si>
+  <si>
     <t>TODO2</t>
   </si>
   <si>
-    <t>The Sangenie</t>
+    <t>Ping-pong</t>
+  </si>
+  <si>
+    <t>Active</t>
   </si>
   <si>
     <t>Create a spreadsheet for BacklogItems</t>
   </si>
   <si>
+    <t>Continuous</t>
+  </si>
+  <si>
+    <t>HOBBY2</t>
+  </si>
+  <si>
     <t>TODO3</t>
   </si>
   <si>
+    <t>Yoga</t>
+  </si>
+  <si>
     <t>Create a spreadsheet for Themes</t>
   </si>
   <si>
-    <t>GOAL34</t>
-  </si>
-  <si>
     <t>TODO4</t>
   </si>
   <si>
+    <t>Read Infinite Jest</t>
+  </si>
+  <si>
     <t>Create a spreadsheet for Goals</t>
   </si>
   <si>
-    <t>Master at least one foreign language</t>
+    <t>Passive</t>
+  </si>
+  <si>
+    <t>OneOff</t>
   </si>
   <si>
     <t>TODO5</t>
   </si>
   <si>
+    <t>HOBBY4</t>
+  </si>
+  <si>
     <t>Create a spreadsheet for Threads</t>
   </si>
   <si>
+    <t>Watch Dr Strangelove</t>
+  </si>
+  <si>
     <t>TODO6</t>
   </si>
   <si>
     <t>Create a spreadsheet for Weaves</t>
   </si>
   <si>
-    <t>GOAL35</t>
-  </si>
-  <si>
     <t>TODO7</t>
   </si>
   <si>
-    <t>Master at least one sport</t>
-  </si>
-  <si>
     <t>Create a spreadsheet for LaserDonuts</t>
   </si>
   <si>
     <t>TODO8</t>
   </si>
   <si>
-    <t>GOAL36</t>
-  </si>
-  <si>
     <t>Create a spreadsheet for Portions</t>
   </si>
   <si>
-    <t>Rekindle your artistic passion</t>
-  </si>
-  <si>
     <t>TODO9</t>
   </si>
   <si>
@@ -690,12 +747,6 @@
     <t>Create a spreadsheet for Hobbies</t>
   </si>
   <si>
-    <t>GOAL37</t>
-  </si>
-  <si>
-    <t>Learn to play an instrument</t>
-  </si>
-  <si>
     <t>TODO11</t>
   </si>
   <si>
@@ -708,18 +759,12 @@
     <t>Create a spreadsheet for WeekDays</t>
   </si>
   <si>
-    <t>GOAL38</t>
-  </si>
-  <si>
     <t>TODO13</t>
   </si>
   <si>
     <t>Create a spreadsheet for Saturdays</t>
   </si>
   <si>
-    <t>Read all of the books in your library, and blog about them</t>
-  </si>
-  <si>
     <t>TODO14</t>
   </si>
   <si>
@@ -735,100 +780,58 @@
     <t>TODO16</t>
   </si>
   <si>
-    <t>Meditate</t>
-  </si>
-  <si>
     <t>Create a spreadsheet for Receipts</t>
   </si>
   <si>
-    <t>GOAL40</t>
+    <t>day</t>
+  </si>
+  <si>
+    <t>current amount</t>
+  </si>
+  <si>
+    <t>goal amount</t>
+  </si>
+  <si>
+    <t>paid in</t>
+  </si>
+  <si>
+    <t>paid out</t>
+  </si>
+  <si>
+    <t>progress</t>
+  </si>
+  <si>
+    <t>FTMONDAY1</t>
+  </si>
+  <si>
+    <t>Frugal</t>
+  </si>
+  <si>
+    <t>tracking</t>
+  </si>
+  <si>
+    <t>purchased item</t>
+  </si>
+  <si>
+    <t>expenditure</t>
+  </si>
+  <si>
+    <t>name of establishment</t>
+  </si>
+  <si>
+    <t>RECEIPT1</t>
+  </si>
+  <si>
+    <t>Green Juice</t>
+  </si>
+  <si>
+    <t>Pret a Manger</t>
   </si>
   <si>
     <t>Create the Ferris Wheel</t>
   </si>
   <si>
     <t>T</t>
-  </si>
-  <si>
-    <t>frequency</t>
-  </si>
-  <si>
-    <t>HOBBY1</t>
-  </si>
-  <si>
-    <t>Ping-pong</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>Continuous</t>
-  </si>
-  <si>
-    <t>HOBBY2</t>
-  </si>
-  <si>
-    <t>Yoga</t>
-  </si>
-  <si>
-    <t>Read Infinite Jest</t>
-  </si>
-  <si>
-    <t>Passive</t>
-  </si>
-  <si>
-    <t>OneOff</t>
-  </si>
-  <si>
-    <t>HOBBY4</t>
-  </si>
-  <si>
-    <t>Watch Dr Strangelove</t>
-  </si>
-  <si>
-    <t>day</t>
-  </si>
-  <si>
-    <t>current amount</t>
-  </si>
-  <si>
-    <t>goal amount</t>
-  </si>
-  <si>
-    <t>paid in</t>
-  </si>
-  <si>
-    <t>paid out</t>
-  </si>
-  <si>
-    <t>progress</t>
-  </si>
-  <si>
-    <t>FTMONDAY1</t>
-  </si>
-  <si>
-    <t>Frugal</t>
-  </si>
-  <si>
-    <t>tracking</t>
-  </si>
-  <si>
-    <t>purchased item</t>
-  </si>
-  <si>
-    <t>expenditure</t>
-  </si>
-  <si>
-    <t>name of establishment</t>
-  </si>
-  <si>
-    <t>RECEIPT1</t>
-  </si>
-  <si>
-    <t>Green Juice</t>
-  </si>
-  <si>
-    <t>Pret a Manger</t>
   </si>
   <si>
     <t>TIMETABLE1</t>
@@ -1051,7 +1054,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2">
@@ -1059,7 +1062,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -1067,23 +1070,23 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1103,7 +1106,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>37</v>
@@ -1117,58 +1120,58 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>81</v>
+        <v>116</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>85</v>
+        <v>125</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>86</v>
+        <v>129</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>88</v>
+        <v>133</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>91</v>
+        <v>136</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6">
@@ -1176,27 +1179,27 @@
         <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>95</v>
+        <v>138</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>97</v>
+        <v>140</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1216,7 +1219,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>37</v>
@@ -1233,36 +1236,36 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4">
@@ -1270,16 +1273,16 @@
         <v>28</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>108</v>
+        <v>132</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1299,7 +1302,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>37</v>
@@ -1308,7 +1311,7 @@
         <v>38</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>129</v>
+        <v>183</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>39</v>
@@ -1317,30 +1320,30 @@
         <v>74</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>130</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>131</v>
+        <v>187</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>133</v>
+        <v>189</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>134</v>
+        <v>190</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>136</v>
+        <v>193</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>137</v>
+        <v>194</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="H2" s="1">
         <v>1.0</v>
@@ -1348,25 +1351,25 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>140</v>
+        <v>182</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>141</v>
+        <v>197</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>142</v>
+        <v>198</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>144</v>
+        <v>199</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>145</v>
+        <v>200</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>137</v>
+        <v>194</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="H3" s="1">
         <v>1.0</v>
@@ -1374,25 +1377,25 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>141</v>
+        <v>197</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>148</v>
+        <v>203</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>149</v>
+        <v>204</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>150</v>
+        <v>206</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>137</v>
+        <v>194</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="H4" s="1">
         <v>2.0</v>
@@ -1418,7 +1421,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>37</v>
@@ -1427,21 +1430,21 @@
         <v>74</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>130</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>140</v>
+        <v>182</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="E2" s="1">
         <v>1.0</v>
@@ -1449,16 +1452,16 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>140</v>
+        <v>182</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="E3" s="1">
         <v>2.0</v>
@@ -1469,13 +1472,13 @@
         <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>179</v>
+        <v>196</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="E4" s="1">
         <v>3.0</v>
@@ -1486,13 +1489,13 @@
         <v>32</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
       <c r="E5" s="1">
         <v>4.0</v>
@@ -1521,7 +1524,7 @@
         <v>38</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>130</v>
+        <v>180</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>74</v>
@@ -1529,226 +1532,274 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>194</v>
+        <v>29</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>209</v>
       </c>
       <c r="D2" s="1">
         <v>1.0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>197</v>
+        <v>29</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>214</v>
       </c>
       <c r="D3" s="1">
         <v>2.0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>198</v>
+        <v>217</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>199</v>
+        <v>29</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>219</v>
       </c>
       <c r="D4" s="1">
         <v>3.0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>201</v>
+        <v>220</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>202</v>
+        <v>29</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>222</v>
       </c>
       <c r="D5" s="1">
         <v>4.0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>204</v>
+        <v>225</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>205</v>
+        <v>29</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>227</v>
       </c>
       <c r="D6" s="1">
         <v>5.0</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>206</v>
+        <v>229</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>207</v>
+        <v>29</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="D7" s="1">
         <v>6.0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>209</v>
+        <v>231</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>211</v>
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>232</v>
       </c>
       <c r="D8" s="1">
         <v>7.0</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>212</v>
+        <v>233</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>214</v>
+        <v>29</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>234</v>
       </c>
       <c r="D9" s="1">
         <v>8.0</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>216</v>
+        <v>235</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>217</v>
+        <v>29</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>236</v>
       </c>
       <c r="D10" s="1">
         <v>9.0</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>218</v>
+        <v>237</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>219</v>
+        <v>29</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>238</v>
       </c>
       <c r="D11" s="1">
         <v>10.0</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>222</v>
+        <v>239</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>223</v>
+        <v>29</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>240</v>
       </c>
       <c r="D12" s="1">
         <v>11.0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>224</v>
+        <v>241</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>225</v>
+        <v>29</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>242</v>
       </c>
       <c r="D13" s="1">
         <v>12.0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>227</v>
+        <v>243</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>228</v>
+        <v>29</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>244</v>
       </c>
       <c r="D14" s="1">
         <v>13.0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>230</v>
+        <v>245</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>231</v>
+        <v>29</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>246</v>
       </c>
       <c r="D15" s="1">
         <v>14.0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>232</v>
+        <v>247</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>233</v>
+        <v>29</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>248</v>
       </c>
       <c r="D16" s="1">
         <v>15.0</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>236</v>
+        <v>29</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>250</v>
       </c>
       <c r="D17" s="1">
         <v>16.0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1768,7 +1819,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>37</v>
@@ -1780,7 +1831,7 @@
         <v>39</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>240</v>
+        <v>208</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>74</v>
@@ -1788,78 +1839,78 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>241</v>
+        <v>210</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>208</v>
+        <v>175</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>242</v>
+        <v>212</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>245</v>
+        <v>216</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>141</v>
+        <v>197</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>246</v>
+        <v>218</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>247</v>
+        <v>221</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>248</v>
+        <v>223</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>249</v>
+        <v>224</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>251</v>
+        <v>228</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>248</v>
+        <v>223</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>249</v>
+        <v>224</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6">
@@ -1882,27 +1933,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>26</v>
@@ -1920,7 +1971,7 @@
         <v>20.0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -1940,33 +1991,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>265</v>
       </c>
       <c r="D2" s="1">
         <v>3.69</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -1986,12 +2037,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>26</v>
@@ -2002,21 +2053,21 @@
         <v>39</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="9" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>74</v>
@@ -2024,7 +2075,7 @@
     </row>
     <row r="6">
       <c r="A6" s="10" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="10">
@@ -2034,15 +2085,15 @@
         <v>610.0</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="C7" s="10">
         <v>610.0</v>
@@ -2054,7 +2105,7 @@
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="10">
@@ -2064,15 +2115,15 @@
         <v>720.0</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>86</v>
+        <v>129</v>
       </c>
       <c r="C9" s="10">
         <v>720.0</v>
@@ -2084,7 +2135,7 @@
     </row>
     <row r="10">
       <c r="A10" s="10" t="s">
-        <v>86</v>
+        <v>129</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="10">
@@ -2094,15 +2145,15 @@
         <v>800.0</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="10" t="s">
-        <v>86</v>
+        <v>129</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="10">
         <v>800.0</v>
@@ -2114,7 +2165,7 @@
     </row>
     <row r="12">
       <c r="A12" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="10">
@@ -2124,15 +2175,15 @@
         <v>1600.0</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="C13" s="10">
         <v>1600.0</v>
@@ -2144,7 +2195,7 @@
     </row>
     <row r="14">
       <c r="A14" s="10" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="10">
@@ -2154,15 +2205,15 @@
         <v>2010.0</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="10" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="C15" s="10">
         <v>2010.0</v>
@@ -2174,7 +2225,7 @@
     </row>
     <row r="16">
       <c r="A16" s="10" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="B16" s="11"/>
       <c r="C16" s="10">
@@ -2184,7 +2235,7 @@
         <v>600.0</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2213,12 +2264,12 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -2230,7 +2281,7 @@
         <v>1.4832288E9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2250,7 +2301,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -2259,21 +2310,21 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C2" s="3">
         <v>1.4516064E9</v>
@@ -2282,13 +2333,13 @@
         <v>1.4521248E9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -2308,16 +2359,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>25</v>
@@ -2328,7 +2379,7 @@
         <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C2" s="4">
         <v>1.4516064E9</v>
@@ -2360,13 +2411,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>25</v>
@@ -2380,7 +2431,7 @@
         <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C2" s="3">
         <v>1.4520384E9</v>
@@ -2392,7 +2443,7 @@
         <v>32</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -2412,16 +2463,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2">
@@ -2429,7 +2480,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C2" s="3">
         <v>1.4521248E9</v>
@@ -2458,7 +2509,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>37</v>
@@ -2472,100 +2523,100 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9">
@@ -2573,13 +2624,13 @@
         <v>68</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>69</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10">
@@ -2602,76 +2653,76 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2717,987 +2768,987 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>78</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="5">
         <v>1.0</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="5">
         <v>2.0</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="5">
         <v>2.0</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="5">
         <v>3.0</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="5">
         <v>3.0</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="5" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="5">
         <v>3.0</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="5">
         <v>1.0</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="5" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="5">
         <v>2.0</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="5">
         <v>1.0</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="8" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="5">
         <v>1.0</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="5" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="5">
         <v>2.0</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>135</v>
+        <v>107</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>138</v>
+        <v>108</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="5">
         <v>1.0</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>143</v>
+        <v>112</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="5">
         <v>1.0</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="5" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="5">
         <v>3.0</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="5">
         <v>2.0</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="F17" s="1">
         <v>4.0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="F18" s="1">
         <v>4.0</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="F19" s="1">
         <v>3.0</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="F20" s="1">
         <v>4.0</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="F21" s="1">
         <v>4.0</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="F22" s="1">
         <v>2.0</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="4" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="F23" s="1">
         <v>2.0</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="4" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="F24" s="1">
         <v>2.0</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="4" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="F25" s="1">
         <v>2.0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="4" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="F26" s="1">
         <v>3.0</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="F27" s="1">
         <v>4.0</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="F28" s="1">
         <v>4.0</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="F29" s="1">
         <v>1.0</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="F30" s="1">
         <v>1.0</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="F31" s="1">
         <v>3.0</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="F32" s="1">
         <v>5.0</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="F33" s="1">
         <v>5.0</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>193</v>
+        <v>171</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="D34" s="1" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="F34" s="1">
         <v>5.0</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>200</v>
+        <v>173</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>203</v>
+        <v>174</v>
       </c>
       <c r="F35" s="1">
         <v>5.0</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>208</v>
+        <v>175</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>210</v>
+        <v>176</v>
       </c>
       <c r="F36" s="1">
         <v>5.0</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>213</v>
+        <v>177</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>215</v>
+        <v>179</v>
       </c>
       <c r="F37" s="1">
         <v>6.0</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>220</v>
+        <v>184</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="F38" s="1">
         <v>6.0</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>226</v>
+        <v>192</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>229</v>
+        <v>195</v>
       </c>
       <c r="F39" s="1">
         <v>6.0</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>141</v>
+        <v>197</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>235</v>
+        <v>202</v>
       </c>
       <c r="F40" s="1">
         <v>6.0</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>238</v>
+        <v>266</v>
       </c>
       <c r="F41" s="1">
         <v>1.0</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>239</v>
+        <v>267</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>